<commit_message>
fix: find si bug
</commit_message>
<xml_diff>
--- a/test/richtext.xlsx
+++ b/test/richtext.xlsx
@@ -20,34 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">This is </t>
-    </r>
     <r>
       <rPr>
         <b val="true"/>
         <sz val="10"/>
-        <color rgb="FFFF3333"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">only one</t>
+      <t xml:space="preserve">B </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> sentence.</t>
+      <t xml:space="preserve">cell</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">C cell</t>
   </si>
 </sst>
 </file>
@@ -62,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -81,9 +78,9 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FFFF3333"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,8 +125,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -142,66 +143,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF3333"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -210,10 +151,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -222,8 +163,11 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>